<commit_message>
Atualização incremental dos arquivos.
</commit_message>
<xml_diff>
--- a/Levantamento Matematica/enade_matematica_2017.xlsx
+++ b/Levantamento Matematica/enade_matematica_2017.xlsx
@@ -17209,7 +17209,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Centro Universitário Estácio de São Paulo</t>
+          <t>CENTRO UNIVERSITÁRIO ESTÁCIO DE SÃO PAULO</t>
         </is>
       </c>
       <c r="E336" t="inlineStr">
@@ -18909,7 +18909,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Centro Universitário de Adamantina</t>
+          <t>CENTRO UNIVERSITÁRIO DE ADAMANTINA</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
@@ -19059,7 +19059,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Faculdade Projeção de Taguatinga Norte</t>
+          <t>FACULDADE PROJEÇÃO DE TAGUATINGA NORTE</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
@@ -25059,7 +25059,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>Centro Universitário UNIFAAT</t>
+          <t>CENTRO UNIVERSITÁRIO UNIFAAT</t>
         </is>
       </c>
       <c r="E493" t="inlineStr">
@@ -25259,7 +25259,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Norte do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO NORTE DO PARANÁ</t>
         </is>
       </c>
       <c r="E497" t="inlineStr">
@@ -25309,7 +25309,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Norte do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO NORTE DO PARANÁ</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
@@ -25509,7 +25509,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>Instituto Federal de Educação, Ciência e Tecnologia do Acre</t>
+          <t>INSTITUTO FEDERAL DE EDUCAÇÃO, CIÊNCIA E TECNOLOGIA DO ACRE</t>
         </is>
       </c>
       <c r="E502" t="inlineStr">
@@ -25609,7 +25609,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO PARANÁ</t>
         </is>
       </c>
       <c r="E504" t="inlineStr">
@@ -25659,7 +25659,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO PARANÁ</t>
         </is>
       </c>
       <c r="E505" t="inlineStr">
@@ -25709,7 +25709,7 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO PARANÁ</t>
         </is>
       </c>
       <c r="E506" t="inlineStr">
@@ -25759,7 +25759,7 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO PARANÁ</t>
         </is>
       </c>
       <c r="E507" t="inlineStr">
@@ -25809,7 +25809,7 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>Universidade Estadual do Paraná</t>
+          <t>UNIVERSIDADE ESTADUAL DO PARANÁ</t>
         </is>
       </c>
       <c r="E508" t="inlineStr">

</xml_diff>